<commit_message>
started cell density analysis
</commit_message>
<xml_diff>
--- a/data/physiology/cell_density/cells.xlsx
+++ b/data/physiology/cell_density/cells.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/physiology/cell_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9FB5F0-9B82-1D43-92D1-FD4D51FEF310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E074AEDB-F6BA-C440-AB16-208D6A6914F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="760" windowWidth="27340" windowHeight="14760" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
+    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="14760" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
   <si>
     <t>Notes</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>POR-R30</t>
+  </si>
+  <si>
+    <t>counted all symbionts</t>
   </si>
 </sst>
 </file>
@@ -383,9 +386,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,7 +706,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,7 +757,7 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="1" t="e">
+      <c r="L2" t="e">
         <f t="shared" ref="L2:L57" si="0">STDEV(E2:J2)/AVERAGE(E2:J2)</f>
         <v>#DIV/0!</v>
       </c>
@@ -764,45 +766,180 @@
       <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B3">
+        <v>20231122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>144</v>
+      </c>
+      <c r="F3">
+        <v>77</v>
+      </c>
+      <c r="G3">
+        <v>111</v>
+      </c>
+      <c r="H3">
+        <v>113</v>
+      </c>
+      <c r="I3">
+        <v>126</v>
+      </c>
+      <c r="J3">
+        <v>105</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>0.19820277188691371</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B4">
+        <v>20231121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>409</v>
+      </c>
+      <c r="F4">
+        <v>401</v>
+      </c>
+      <c r="G4">
+        <v>468</v>
+      </c>
+      <c r="H4">
+        <v>404</v>
+      </c>
+      <c r="I4">
+        <v>446</v>
+      </c>
+      <c r="J4">
+        <v>470</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>7.4506771552625264E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B5">
+        <v>20231123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>212</v>
+      </c>
+      <c r="F5">
+        <v>199</v>
+      </c>
+      <c r="G5">
+        <v>180</v>
+      </c>
+      <c r="H5">
+        <v>213</v>
+      </c>
+      <c r="I5">
+        <v>189</v>
+      </c>
+      <c r="J5">
+        <v>208</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>6.6982727186520069E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B6">
+        <v>20231122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>346</v>
+      </c>
+      <c r="F6">
+        <v>305</v>
+      </c>
+      <c r="G6">
+        <v>304</v>
+      </c>
+      <c r="H6">
+        <v>303</v>
+      </c>
+      <c r="I6">
+        <v>398</v>
+      </c>
+      <c r="J6">
+        <v>327</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.11254290416579298</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B7">
+        <v>20231121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>269</v>
+      </c>
+      <c r="F7">
+        <v>287</v>
+      </c>
+      <c r="G7">
+        <v>386</v>
+      </c>
+      <c r="H7">
+        <v>296</v>
+      </c>
+      <c r="I7">
+        <v>259</v>
+      </c>
+      <c r="J7">
+        <v>291</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.15215817515106891</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -836,7 +973,7 @@
       <c r="J8">
         <v>231</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8">
         <f t="shared" ref="L8" si="1">STDEV(E8:J8)/AVERAGE(E8:J8)</f>
         <v>5.4499681837948573E-2</v>
       </c>
@@ -845,25 +982,79 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B9">
+        <v>20231121</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>193</v>
+      </c>
+      <c r="F9">
+        <v>202</v>
+      </c>
+      <c r="G9">
+        <v>177</v>
+      </c>
+      <c r="H9">
+        <v>209</v>
+      </c>
+      <c r="I9">
+        <v>206</v>
+      </c>
+      <c r="J9">
+        <v>216</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>6.8874898138469989E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B10">
+        <v>20221122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>145</v>
+      </c>
+      <c r="G10">
+        <v>226</v>
+      </c>
+      <c r="H10">
+        <v>187</v>
+      </c>
+      <c r="I10">
+        <v>163</v>
+      </c>
+      <c r="J10">
+        <v>138</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0.19727327824611601</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="1" t="e">
+      <c r="L11" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -872,7 +1063,7 @@
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="1" t="e">
+      <c r="L12" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -881,25 +1072,79 @@
       <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B13">
+        <v>20231121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>360</v>
+      </c>
+      <c r="F13">
+        <v>350</v>
+      </c>
+      <c r="G13">
+        <v>377</v>
+      </c>
+      <c r="H13">
+        <v>354</v>
+      </c>
+      <c r="I13">
+        <v>411</v>
+      </c>
+      <c r="J13">
+        <v>398</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>6.6613311982916243E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B14">
+        <v>20231120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>121</v>
+      </c>
+      <c r="F14">
+        <v>139</v>
+      </c>
+      <c r="G14">
+        <v>128</v>
+      </c>
+      <c r="H14">
+        <v>138</v>
+      </c>
+      <c r="I14">
+        <v>132</v>
+      </c>
+      <c r="J14">
+        <v>140</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>5.6265524613141972E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="1" t="e">
+      <c r="L15" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -908,7 +1153,7 @@
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="1" t="e">
+      <c r="L16" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -917,61 +1162,223 @@
       <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B17">
+        <v>20231123</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>176</v>
+      </c>
+      <c r="F17">
+        <v>213</v>
+      </c>
+      <c r="G17">
+        <v>183</v>
+      </c>
+      <c r="H17">
+        <v>193</v>
+      </c>
+      <c r="I17">
+        <v>197</v>
+      </c>
+      <c r="J17">
+        <v>151</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0.11388578756765692</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B18">
+        <v>20231121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>132</v>
+      </c>
+      <c r="F18">
+        <v>157</v>
+      </c>
+      <c r="G18">
+        <v>154</v>
+      </c>
+      <c r="H18">
+        <v>169</v>
+      </c>
+      <c r="I18">
+        <v>160</v>
+      </c>
+      <c r="J18">
+        <v>161</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>8.0809174752153157E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="L19" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B19">
+        <v>20231123</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>115</v>
+      </c>
+      <c r="F19">
+        <v>136</v>
+      </c>
+      <c r="G19">
+        <v>137</v>
+      </c>
+      <c r="H19">
+        <v>131</v>
+      </c>
+      <c r="I19">
+        <v>161</v>
+      </c>
+      <c r="J19">
+        <v>154</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>0.11873773258001587</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B20">
+        <v>20231121</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>215</v>
+      </c>
+      <c r="F20">
+        <v>283</v>
+      </c>
+      <c r="G20">
+        <v>297</v>
+      </c>
+      <c r="H20">
+        <v>243</v>
+      </c>
+      <c r="I20">
+        <v>262</v>
+      </c>
+      <c r="J20">
+        <v>285</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0.11651478383524048</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B21">
+        <v>20231123</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>174</v>
+      </c>
+      <c r="F21">
+        <v>210</v>
+      </c>
+      <c r="G21">
+        <v>246</v>
+      </c>
+      <c r="H21">
+        <v>251</v>
+      </c>
+      <c r="I21">
+        <v>224</v>
+      </c>
+      <c r="J21">
+        <v>189</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>0.14242304097918831</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B22">
+        <v>20231121</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>130</v>
+      </c>
+      <c r="F22">
+        <v>177</v>
+      </c>
+      <c r="G22">
+        <v>96</v>
+      </c>
+      <c r="H22">
+        <v>98</v>
+      </c>
+      <c r="I22">
+        <v>118</v>
+      </c>
+      <c r="J22">
+        <v>123</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0.23827249330995171</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="1" t="e">
+      <c r="L23" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -980,34 +1387,115 @@
       <c r="A24" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B24">
+        <v>20231122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>211</v>
+      </c>
+      <c r="F24">
+        <v>184</v>
+      </c>
+      <c r="G24">
+        <v>193</v>
+      </c>
+      <c r="H24">
+        <v>241</v>
+      </c>
+      <c r="I24">
+        <v>269</v>
+      </c>
+      <c r="J24">
+        <v>253</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>0.15225886440196346</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>43</v>
       </c>
-      <c r="L25" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B25">
+        <v>20231120</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>106</v>
+      </c>
+      <c r="F25">
+        <v>107</v>
+      </c>
+      <c r="G25">
+        <v>111</v>
+      </c>
+      <c r="H25">
+        <v>118</v>
+      </c>
+      <c r="I25">
+        <v>95</v>
+      </c>
+      <c r="J25">
+        <v>113</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>7.2369858709991575E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>44</v>
       </c>
-      <c r="L26" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B26">
+        <v>20231120</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>169</v>
+      </c>
+      <c r="F26">
+        <v>136</v>
+      </c>
+      <c r="G26">
+        <v>108</v>
+      </c>
+      <c r="H26">
+        <v>112</v>
+      </c>
+      <c r="I26">
+        <v>150</v>
+      </c>
+      <c r="J26">
+        <v>177</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>0.20190522798354155</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>45</v>
       </c>
-      <c r="L27" s="1" t="e">
+      <c r="L27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1016,9 +1504,36 @@
       <c r="A28" t="s">
         <v>46</v>
       </c>
-      <c r="L28" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B28">
+        <v>20231122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>232</v>
+      </c>
+      <c r="F28">
+        <v>225</v>
+      </c>
+      <c r="G28">
+        <v>217</v>
+      </c>
+      <c r="H28">
+        <v>209</v>
+      </c>
+      <c r="I28">
+        <v>219</v>
+      </c>
+      <c r="J28">
+        <v>258</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>7.583445820933328E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1052,7 +1567,7 @@
       <c r="J29">
         <v>541</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L29">
         <f t="shared" ref="L29" si="2">STDEV(E29:J29)/AVERAGE(E29:J29)</f>
         <v>4.3655366029142065E-2</v>
       </c>
@@ -1061,25 +1576,79 @@
       <c r="A30" t="s">
         <v>47</v>
       </c>
-      <c r="L30" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B30">
+        <v>20231123</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>184</v>
+      </c>
+      <c r="F30">
+        <v>176</v>
+      </c>
+      <c r="G30">
+        <v>210</v>
+      </c>
+      <c r="H30">
+        <v>183</v>
+      </c>
+      <c r="I30">
+        <v>193</v>
+      </c>
+      <c r="J30">
+        <v>191</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>6.1968776097476204E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>48</v>
       </c>
-      <c r="L31" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B31">
+        <v>20231121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>368</v>
+      </c>
+      <c r="F31">
+        <v>436</v>
+      </c>
+      <c r="G31">
+        <v>407</v>
+      </c>
+      <c r="H31">
+        <v>396</v>
+      </c>
+      <c r="I31">
+        <v>401</v>
+      </c>
+      <c r="J31">
+        <v>387</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>5.6585058894035339E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
-      <c r="L32" s="1" t="e">
+      <c r="L32" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1088,25 +1657,79 @@
       <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="L33" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B33">
+        <v>20231121</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>212</v>
+      </c>
+      <c r="F33">
+        <v>233</v>
+      </c>
+      <c r="G33">
+        <v>218</v>
+      </c>
+      <c r="H33">
+        <v>200</v>
+      </c>
+      <c r="I33">
+        <v>212</v>
+      </c>
+      <c r="J33">
+        <v>204</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>5.4580382299483879E-2</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>51</v>
       </c>
-      <c r="L34" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B34">
+        <v>20231122</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>209</v>
+      </c>
+      <c r="F34">
+        <v>153</v>
+      </c>
+      <c r="G34">
+        <v>194</v>
+      </c>
+      <c r="H34">
+        <v>193</v>
+      </c>
+      <c r="I34">
+        <v>193</v>
+      </c>
+      <c r="J34">
+        <v>226</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>0.12433912367739489</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>52</v>
       </c>
-      <c r="L35" s="1" t="e">
+      <c r="L35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1115,16 +1738,43 @@
       <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="L36" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B36">
+        <v>20231120</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>436</v>
+      </c>
+      <c r="F36">
+        <v>495</v>
+      </c>
+      <c r="G36">
+        <v>484</v>
+      </c>
+      <c r="H36">
+        <v>522</v>
+      </c>
+      <c r="I36">
+        <v>491</v>
+      </c>
+      <c r="J36">
+        <v>509</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>6.0336517517073147E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="L37" s="1" t="e">
+      <c r="L37" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1133,25 +1783,79 @@
       <c r="A38" t="s">
         <v>55</v>
       </c>
-      <c r="L38" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B38">
+        <v>20231120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>344</v>
+      </c>
+      <c r="F38">
+        <v>384</v>
+      </c>
+      <c r="G38">
+        <v>404</v>
+      </c>
+      <c r="H38">
+        <v>465</v>
+      </c>
+      <c r="I38">
+        <v>359</v>
+      </c>
+      <c r="J38">
+        <v>398</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>0.10793020709906821</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>56</v>
       </c>
-      <c r="L39" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B39">
+        <v>20231120</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>127</v>
+      </c>
+      <c r="F39">
+        <v>106</v>
+      </c>
+      <c r="G39">
+        <v>103</v>
+      </c>
+      <c r="H39">
+        <v>100</v>
+      </c>
+      <c r="I39">
+        <v>96</v>
+      </c>
+      <c r="J39">
+        <v>101</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>0.10465244835909401</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="L40" s="1" t="e">
+      <c r="L40" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1160,25 +1864,79 @@
       <c r="A41" t="s">
         <v>58</v>
       </c>
-      <c r="L41" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B41">
+        <v>20231122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>162</v>
+      </c>
+      <c r="F41">
+        <v>175</v>
+      </c>
+      <c r="G41">
+        <v>176</v>
+      </c>
+      <c r="H41">
+        <v>171</v>
+      </c>
+      <c r="I41">
+        <v>167</v>
+      </c>
+      <c r="J41">
+        <v>132</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>0.10032602714904687</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="L42" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B42">
+        <v>20231122</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>166</v>
+      </c>
+      <c r="F42">
+        <v>213</v>
+      </c>
+      <c r="G42">
+        <v>164</v>
+      </c>
+      <c r="H42">
+        <v>184</v>
+      </c>
+      <c r="I42">
+        <v>193</v>
+      </c>
+      <c r="J42">
+        <v>181</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>9.9101682746700032E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>60</v>
       </c>
-      <c r="L43" s="1" t="e">
+      <c r="L43" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1187,7 +1945,7 @@
       <c r="A44" t="s">
         <v>61</v>
       </c>
-      <c r="L44" s="1" t="e">
+      <c r="L44" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1196,80 +1954,214 @@
       <c r="A45" t="s">
         <v>62</v>
       </c>
-      <c r="L45" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B45">
+        <v>20231121</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>134</v>
+      </c>
+      <c r="F45">
+        <v>170</v>
+      </c>
+      <c r="G45">
+        <v>146</v>
+      </c>
+      <c r="H45">
+        <v>150</v>
+      </c>
+      <c r="I45">
+        <v>161</v>
+      </c>
+      <c r="J45">
+        <v>168</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>9.0273601618578933E-2</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>63</v>
       </c>
-      <c r="L46" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B46">
+        <v>20231123</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>131</v>
+      </c>
+      <c r="F46">
+        <v>144</v>
+      </c>
+      <c r="G46">
+        <v>99</v>
+      </c>
+      <c r="H46">
+        <v>170</v>
+      </c>
+      <c r="I46">
+        <v>156</v>
+      </c>
+      <c r="J46">
+        <v>157</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>0.17641921772370969</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
-      <c r="L47" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B47">
+        <v>20231123</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>131</v>
+      </c>
+      <c r="F47">
+        <v>109</v>
+      </c>
+      <c r="G47">
+        <v>90</v>
+      </c>
+      <c r="H47">
+        <v>111</v>
+      </c>
+      <c r="I47">
+        <v>94</v>
+      </c>
+      <c r="J47">
+        <v>99</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>0.14083680916815181</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
-      <c r="L48" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B48">
+        <v>20231123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>139</v>
+      </c>
+      <c r="F48">
+        <v>175</v>
+      </c>
+      <c r="G48">
+        <v>149</v>
+      </c>
+      <c r="H48">
+        <v>184</v>
+      </c>
+      <c r="I48">
+        <v>136</v>
+      </c>
+      <c r="J48">
+        <v>159</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>0.12370469693054995</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
-      <c r="L49" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B49">
+        <v>20231122</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <v>89</v>
+      </c>
+      <c r="F49">
+        <v>73</v>
+      </c>
+      <c r="G49">
+        <v>69</v>
+      </c>
+      <c r="H49">
+        <v>81</v>
+      </c>
+      <c r="I49">
+        <v>62</v>
+      </c>
+      <c r="J49">
+        <v>68</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>0.13291157197422951</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50">
         <v>20231119</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1">
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
         <v>125</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50">
         <v>123</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50">
         <v>112</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50">
         <v>137</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50">
         <v>137</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50">
         <v>152</v>
       </c>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1">
+      <c r="L50">
         <f>STDEV(E50:J50)/AVERAGE(E50:J50)</f>
         <v>0.10654257296102536</v>
       </c>
@@ -1278,7 +2170,7 @@
       <c r="A51" t="s">
         <v>67</v>
       </c>
-      <c r="L51" s="1" t="e">
+      <c r="L51" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1287,18 +2179,72 @@
       <c r="A52" t="s">
         <v>68</v>
       </c>
-      <c r="L52" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B52">
+        <v>20231120</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>123</v>
+      </c>
+      <c r="F52">
+        <v>157</v>
+      </c>
+      <c r="G52">
+        <v>179</v>
+      </c>
+      <c r="H52">
+        <v>145</v>
+      </c>
+      <c r="I52">
+        <v>160</v>
+      </c>
+      <c r="J52">
+        <v>151</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>0.12117848270541855</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>69</v>
       </c>
-      <c r="L53" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B53">
+        <v>20231120</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>125</v>
+      </c>
+      <c r="F53">
+        <v>152</v>
+      </c>
+      <c r="G53">
+        <v>113</v>
+      </c>
+      <c r="H53">
+        <v>120</v>
+      </c>
+      <c r="I53">
+        <v>143</v>
+      </c>
+      <c r="J53">
+        <v>127</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="0"/>
+        <v>0.11284382043625998</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -1332,7 +2278,7 @@
       <c r="J54">
         <v>301</v>
       </c>
-      <c r="L54" s="1">
+      <c r="L54">
         <f t="shared" ref="L54" si="3">STDEV(E54:J54)/AVERAGE(E54:J54)</f>
         <v>8.723379711878837E-2</v>
       </c>
@@ -1341,9 +2287,36 @@
       <c r="A55" t="s">
         <v>71</v>
       </c>
-      <c r="L55" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B55">
+        <v>20231122</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>107</v>
+      </c>
+      <c r="F55">
+        <v>115</v>
+      </c>
+      <c r="G55">
+        <v>108</v>
+      </c>
+      <c r="H55">
+        <v>116</v>
+      </c>
+      <c r="I55">
+        <v>127</v>
+      </c>
+      <c r="J55">
+        <v>131</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="0"/>
+        <v>8.3621231338569246E-2</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -1377,7 +2350,7 @@
       <c r="J56">
         <v>150</v>
       </c>
-      <c r="L56" s="1">
+      <c r="L56">
         <f t="shared" si="0"/>
         <v>0.10219540708524746</v>
       </c>
@@ -1386,34 +2359,118 @@
       <c r="A57" t="s">
         <v>73</v>
       </c>
-      <c r="L57" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B57">
+        <v>20231120</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57">
+        <v>9</v>
+      </c>
+      <c r="E57">
+        <v>59</v>
+      </c>
+      <c r="F57">
+        <v>45</v>
+      </c>
+      <c r="G57">
+        <v>64</v>
+      </c>
+      <c r="H57">
+        <v>75</v>
+      </c>
+      <c r="I57">
+        <v>69</v>
+      </c>
+      <c r="J57">
+        <v>70</v>
+      </c>
+      <c r="K57" t="s">
+        <v>104</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="0"/>
+        <v>0.16731005262730159</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>74</v>
       </c>
-      <c r="L58" s="1" t="e">
+      <c r="B58">
+        <v>20231120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>142</v>
+      </c>
+      <c r="F58">
+        <v>169</v>
+      </c>
+      <c r="G58">
+        <v>161</v>
+      </c>
+      <c r="H58">
+        <v>151</v>
+      </c>
+      <c r="I58">
+        <v>190</v>
+      </c>
+      <c r="J58">
+        <v>152</v>
+      </c>
+      <c r="L58">
         <f t="shared" ref="L58:L91" si="4">STDEV(E58:J58)/AVERAGE(E58:J58)</f>
-        <v>#DIV/0!</v>
+        <v>0.10576651333842681</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>75</v>
       </c>
-      <c r="L59" s="1" t="e">
+      <c r="B59">
+        <v>20231120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>190</v>
+      </c>
+      <c r="F59">
+        <v>199</v>
+      </c>
+      <c r="G59">
+        <v>176</v>
+      </c>
+      <c r="H59">
+        <v>197</v>
+      </c>
+      <c r="I59">
+        <v>177</v>
+      </c>
+      <c r="J59">
+        <v>192</v>
+      </c>
+      <c r="L59">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.2275507824191034E-2</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>76</v>
       </c>
-      <c r="L60" s="1" t="e">
+      <c r="L60" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1422,7 +2479,7 @@
       <c r="A61" t="s">
         <v>77</v>
       </c>
-      <c r="L61" s="1" t="e">
+      <c r="L61" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1431,16 +2488,43 @@
       <c r="A62" t="s">
         <v>78</v>
       </c>
-      <c r="L62" s="1" t="e">
+      <c r="B62">
+        <v>20231122</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>119</v>
+      </c>
+      <c r="F62">
+        <v>113</v>
+      </c>
+      <c r="G62">
+        <v>113</v>
+      </c>
+      <c r="H62">
+        <v>121</v>
+      </c>
+      <c r="I62">
+        <v>142</v>
+      </c>
+      <c r="J62">
+        <v>119</v>
+      </c>
+      <c r="L62">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>8.8645564875478866E-2</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>79</v>
       </c>
-      <c r="L63" s="1" t="e">
+      <c r="L63" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1476,7 +2560,7 @@
       <c r="J64">
         <v>165</v>
       </c>
-      <c r="L64" s="1">
+      <c r="L64">
         <f t="shared" si="4"/>
         <v>9.362877418437475E-2</v>
       </c>
@@ -1485,7 +2569,7 @@
       <c r="A65" t="s">
         <v>80</v>
       </c>
-      <c r="L65" s="1" t="e">
+      <c r="L65" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1494,7 +2578,7 @@
       <c r="A66" t="s">
         <v>81</v>
       </c>
-      <c r="L66" s="1" t="e">
+      <c r="L66" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1503,7 +2587,7 @@
       <c r="A67" t="s">
         <v>82</v>
       </c>
-      <c r="L67" s="1" t="e">
+      <c r="L67" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1512,7 +2596,7 @@
       <c r="A68" t="s">
         <v>83</v>
       </c>
-      <c r="L68" s="1" t="e">
+      <c r="L68" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1521,36 +2605,144 @@
       <c r="A69" t="s">
         <v>84</v>
       </c>
-      <c r="L69" s="1" t="e">
+      <c r="B69">
+        <v>20231121</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>199</v>
+      </c>
+      <c r="F69">
+        <v>223</v>
+      </c>
+      <c r="G69">
+        <v>205</v>
+      </c>
+      <c r="H69">
+        <v>229</v>
+      </c>
+      <c r="I69">
+        <v>250</v>
+      </c>
+      <c r="J69">
+        <v>292</v>
+      </c>
+      <c r="L69">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.1465022575094298</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>85</v>
       </c>
-      <c r="L70" s="1" t="e">
+      <c r="B70">
+        <v>20231120</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>197</v>
+      </c>
+      <c r="F70">
+        <v>189</v>
+      </c>
+      <c r="G70">
+        <v>252</v>
+      </c>
+      <c r="H70">
+        <v>202</v>
+      </c>
+      <c r="I70">
+        <v>235</v>
+      </c>
+      <c r="J70">
+        <v>213</v>
+      </c>
+      <c r="L70">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.11298544684787293</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>86</v>
       </c>
-      <c r="L71" s="1" t="e">
+      <c r="B71">
+        <v>20231122</v>
+      </c>
+      <c r="C71" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>311</v>
+      </c>
+      <c r="F71">
+        <v>346</v>
+      </c>
+      <c r="G71">
+        <v>350</v>
+      </c>
+      <c r="H71">
+        <v>340</v>
+      </c>
+      <c r="I71">
+        <v>301</v>
+      </c>
+      <c r="J71">
+        <v>350</v>
+      </c>
+      <c r="L71">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>6.4463220972966917E-2</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>87</v>
       </c>
-      <c r="L72" s="1" t="e">
+      <c r="B72">
+        <v>20231123</v>
+      </c>
+      <c r="C72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>219</v>
+      </c>
+      <c r="F72">
+        <v>225</v>
+      </c>
+      <c r="G72">
+        <v>275</v>
+      </c>
+      <c r="H72">
+        <v>248</v>
+      </c>
+      <c r="I72">
+        <v>207</v>
+      </c>
+      <c r="J72">
+        <v>224</v>
+      </c>
+      <c r="L72">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.10523339094439083</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -1584,7 +2776,7 @@
       <c r="J73">
         <v>153</v>
       </c>
-      <c r="L73" s="1">
+      <c r="L73">
         <f t="shared" si="4"/>
         <v>8.3447685593838444E-2</v>
       </c>
@@ -1593,25 +2785,79 @@
       <c r="A74" t="s">
         <v>88</v>
       </c>
-      <c r="L74" s="1" t="e">
+      <c r="B74">
+        <v>20231120</v>
+      </c>
+      <c r="C74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74">
+        <v>9</v>
+      </c>
+      <c r="E74">
+        <v>90</v>
+      </c>
+      <c r="F74">
+        <v>92</v>
+      </c>
+      <c r="G74">
+        <v>108</v>
+      </c>
+      <c r="H74">
+        <v>84</v>
+      </c>
+      <c r="I74">
+        <v>92</v>
+      </c>
+      <c r="J74">
+        <v>112</v>
+      </c>
+      <c r="L74">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.11478296741295096</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>89</v>
       </c>
-      <c r="L75" s="1" t="e">
+      <c r="B75">
+        <v>20231123</v>
+      </c>
+      <c r="C75" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75">
+        <v>9</v>
+      </c>
+      <c r="E75">
+        <v>94</v>
+      </c>
+      <c r="F75">
+        <v>132</v>
+      </c>
+      <c r="G75">
+        <v>128</v>
+      </c>
+      <c r="H75">
+        <v>158</v>
+      </c>
+      <c r="I75">
+        <v>143</v>
+      </c>
+      <c r="J75">
+        <v>137</v>
+      </c>
+      <c r="L75">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.16184485082698888</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>90</v>
       </c>
-      <c r="L76" s="1" t="e">
+      <c r="L76" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1647,7 +2893,7 @@
       <c r="J77">
         <v>112</v>
       </c>
-      <c r="L77" s="1">
+      <c r="L77">
         <f t="shared" si="4"/>
         <v>0.10729815265965958</v>
       </c>
@@ -1656,7 +2902,7 @@
       <c r="A78" t="s">
         <v>91</v>
       </c>
-      <c r="L78" s="1" t="e">
+      <c r="L78" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1665,25 +2911,79 @@
       <c r="A79" t="s">
         <v>92</v>
       </c>
-      <c r="L79" s="1" t="e">
+      <c r="B79">
+        <v>20231121</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>143</v>
+      </c>
+      <c r="F79">
+        <v>134</v>
+      </c>
+      <c r="G79">
+        <v>122</v>
+      </c>
+      <c r="H79">
+        <v>136</v>
+      </c>
+      <c r="I79">
+        <v>140</v>
+      </c>
+      <c r="J79">
+        <v>141</v>
+      </c>
+      <c r="L79">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.5998331660764032E-2</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>93</v>
       </c>
-      <c r="L80" s="1" t="e">
+      <c r="B80">
+        <v>20231123</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80">
+        <v>129</v>
+      </c>
+      <c r="F80">
+        <v>114</v>
+      </c>
+      <c r="G80">
+        <v>145</v>
+      </c>
+      <c r="H80">
+        <v>143</v>
+      </c>
+      <c r="I80">
+        <v>145</v>
+      </c>
+      <c r="J80">
+        <v>163</v>
+      </c>
+      <c r="L80">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.11901536741848444</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>94</v>
       </c>
-      <c r="L81" s="1" t="e">
+      <c r="L81" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1692,25 +2992,79 @@
       <c r="A82" t="s">
         <v>95</v>
       </c>
-      <c r="L82" s="1" t="e">
+      <c r="B82">
+        <v>20231121</v>
+      </c>
+      <c r="C82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>167</v>
+      </c>
+      <c r="F82">
+        <v>182</v>
+      </c>
+      <c r="G82">
+        <v>169</v>
+      </c>
+      <c r="H82">
+        <v>165</v>
+      </c>
+      <c r="I82">
+        <v>196</v>
+      </c>
+      <c r="J82">
+        <v>222</v>
+      </c>
+      <c r="L82">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.12101283424380715</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>96</v>
       </c>
-      <c r="L83" s="1" t="e">
+      <c r="B83">
+        <v>20231121</v>
+      </c>
+      <c r="C83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>193</v>
+      </c>
+      <c r="F83">
+        <v>175</v>
+      </c>
+      <c r="G83">
+        <v>130</v>
+      </c>
+      <c r="H83">
+        <v>141</v>
+      </c>
+      <c r="I83">
+        <v>139</v>
+      </c>
+      <c r="J83">
+        <v>174</v>
+      </c>
+      <c r="L83">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.15947578484383507</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>97</v>
       </c>
-      <c r="L84" s="1" t="e">
+      <c r="L84" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1746,7 +3100,7 @@
       <c r="J85">
         <v>189</v>
       </c>
-      <c r="L85" s="1">
+      <c r="L85">
         <f t="shared" ref="L85" si="5">STDEV(E85:J85)/AVERAGE(E85:J85)</f>
         <v>3.5990774094480579E-2</v>
       </c>
@@ -1755,34 +3109,115 @@
       <c r="A86" t="s">
         <v>98</v>
       </c>
-      <c r="L86" s="1" t="e">
+      <c r="B86">
+        <v>20231123</v>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <v>204</v>
+      </c>
+      <c r="F86">
+        <v>185</v>
+      </c>
+      <c r="G86">
+        <v>189</v>
+      </c>
+      <c r="H86">
+        <v>162</v>
+      </c>
+      <c r="I86">
+        <v>156</v>
+      </c>
+      <c r="J86">
+        <v>176</v>
+      </c>
+      <c r="L86">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>9.9725341235627082E-2</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>99</v>
       </c>
-      <c r="L87" s="1" t="e">
+      <c r="B87">
+        <v>20231122</v>
+      </c>
+      <c r="C87" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87">
+        <v>127</v>
+      </c>
+      <c r="F87">
+        <v>117</v>
+      </c>
+      <c r="G87">
+        <v>128</v>
+      </c>
+      <c r="H87">
+        <v>116</v>
+      </c>
+      <c r="I87">
+        <v>102</v>
+      </c>
+      <c r="J87">
+        <v>119</v>
+      </c>
+      <c r="L87">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>7.9641634590415261E-2</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>100</v>
       </c>
-      <c r="L88" s="1" t="e">
+      <c r="B88">
+        <v>20231120</v>
+      </c>
+      <c r="C88" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>131</v>
+      </c>
+      <c r="F88">
+        <v>168</v>
+      </c>
+      <c r="G88">
+        <v>187</v>
+      </c>
+      <c r="H88">
+        <v>174</v>
+      </c>
+      <c r="I88">
+        <v>139</v>
+      </c>
+      <c r="J88">
+        <v>138</v>
+      </c>
+      <c r="L88">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.14788515972771957</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>101</v>
       </c>
-      <c r="L89" s="1" t="e">
+      <c r="L89" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1791,7 +3226,7 @@
       <c r="A90" t="s">
         <v>102</v>
       </c>
-      <c r="L90" s="1" t="e">
+      <c r="L90" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -1800,9 +3235,36 @@
       <c r="A91" t="s">
         <v>103</v>
       </c>
-      <c r="L91" s="1" t="e">
+      <c r="B91">
+        <v>20231122</v>
+      </c>
+      <c r="C91" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>288</v>
+      </c>
+      <c r="F91">
+        <v>280</v>
+      </c>
+      <c r="G91">
+        <v>214</v>
+      </c>
+      <c r="H91">
+        <v>289</v>
+      </c>
+      <c r="I91">
+        <v>298</v>
+      </c>
+      <c r="J91">
+        <v>347</v>
+      </c>
+      <c r="L91">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.14914954435482167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new cell density data
</commit_message>
<xml_diff>
--- a/data/physiology/cell_density/cells.xlsx
+++ b/data/physiology/cell_density/cells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/physiology/cell_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E074AEDB-F6BA-C440-AB16-208D6A6914F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0C3974-F281-6444-A904-A7050ED3B834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="14760" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="105">
   <si>
     <t>Notes</t>
   </si>
@@ -705,8 +705,8 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1648,9 +1648,36 @@
       <c r="A32" t="s">
         <v>49</v>
       </c>
-      <c r="L32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B32">
+        <v>20231125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>439</v>
+      </c>
+      <c r="F32">
+        <v>462</v>
+      </c>
+      <c r="G32">
+        <v>477</v>
+      </c>
+      <c r="H32">
+        <v>554</v>
+      </c>
+      <c r="I32">
+        <v>513</v>
+      </c>
+      <c r="J32">
+        <v>476</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>8.3764782556768433E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1855,9 +1882,36 @@
       <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="L40" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B40">
+        <v>20231125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>206</v>
+      </c>
+      <c r="F40">
+        <v>196</v>
+      </c>
+      <c r="G40">
+        <v>293</v>
+      </c>
+      <c r="H40">
+        <v>225</v>
+      </c>
+      <c r="I40">
+        <v>215</v>
+      </c>
+      <c r="J40">
+        <v>222</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>0.15222912739452182</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2524,9 +2578,36 @@
       <c r="A63" t="s">
         <v>79</v>
       </c>
-      <c r="L63" t="e">
+      <c r="B63">
+        <v>20231125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>143</v>
+      </c>
+      <c r="F63">
+        <v>109</v>
+      </c>
+      <c r="G63">
+        <v>123</v>
+      </c>
+      <c r="H63">
+        <v>136</v>
+      </c>
+      <c r="I63">
+        <v>102</v>
+      </c>
+      <c r="J63">
+        <v>100</v>
+      </c>
+      <c r="L63">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.15197827406994388</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -2983,9 +3064,36 @@
       <c r="A81" t="s">
         <v>94</v>
       </c>
-      <c r="L81" t="e">
+      <c r="B81">
+        <v>20231125</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>180</v>
+      </c>
+      <c r="F81">
+        <v>213</v>
+      </c>
+      <c r="G81">
+        <v>156</v>
+      </c>
+      <c r="H81">
+        <v>172</v>
+      </c>
+      <c r="I81">
+        <v>173</v>
+      </c>
+      <c r="J81">
+        <v>178</v>
+      </c>
+      <c r="L81">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.10534686366530677</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added 11/25 cell density data
</commit_message>
<xml_diff>
--- a/data/physiology/cell_density/cells.xlsx
+++ b/data/physiology/cell_density/cells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/physiology/cell_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0C3974-F281-6444-A904-A7050ED3B834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A43D64-A6FD-9341-B0DD-145A21878C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="14760" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>Notes</t>
   </si>
@@ -705,8 +705,8 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,9 +1153,36 @@
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="L16" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B16">
+        <v>20231125</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>326</v>
+      </c>
+      <c r="F16">
+        <v>284</v>
+      </c>
+      <c r="G16">
+        <v>299</v>
+      </c>
+      <c r="H16">
+        <v>334</v>
+      </c>
+      <c r="I16">
+        <v>278</v>
+      </c>
+      <c r="J16">
+        <v>256</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.1003993477743943</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added pr ratio and p gross calculations
</commit_message>
<xml_diff>
--- a/data/physiology/cell_density/cells.xlsx
+++ b/data/physiology/cell_density/cells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/physiology/cell_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A43D64-A6FD-9341-B0DD-145A21878C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC869CC-576C-5547-8A6B-A04A1AD34CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="14760" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
+    <workbookView xWindow="12340" yWindow="760" windowWidth="18400" windowHeight="17580" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
   <si>
     <t>Notes</t>
   </si>
@@ -706,7 +706,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1522,9 +1522,36 @@
       <c r="A27" t="s">
         <v>45</v>
       </c>
-      <c r="L27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B27">
+        <v>20231126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>279</v>
+      </c>
+      <c r="F27">
+        <v>289</v>
+      </c>
+      <c r="G27">
+        <v>315</v>
+      </c>
+      <c r="H27">
+        <v>283</v>
+      </c>
+      <c r="I27">
+        <v>306</v>
+      </c>
+      <c r="J27">
+        <v>326</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>6.309273271690298E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1783,9 +1810,36 @@
       <c r="A35" t="s">
         <v>52</v>
       </c>
-      <c r="L35" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B35">
+        <v>20231126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>210</v>
+      </c>
+      <c r="F35">
+        <v>163</v>
+      </c>
+      <c r="G35">
+        <v>183</v>
+      </c>
+      <c r="H35">
+        <v>188</v>
+      </c>
+      <c r="I35">
+        <v>189</v>
+      </c>
+      <c r="J35">
+        <v>171</v>
+      </c>
+      <c r="L35">
+        <f>STDEV(F35:J35)/AVERAGE(F35:J35)</f>
+        <v>6.3571687867484655E-2</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -1828,9 +1882,36 @@
       <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="L37" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B37">
+        <v>20231126</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>213</v>
+      </c>
+      <c r="F37">
+        <v>171</v>
+      </c>
+      <c r="G37">
+        <v>201</v>
+      </c>
+      <c r="H37">
+        <v>253</v>
+      </c>
+      <c r="I37">
+        <v>226</v>
+      </c>
+      <c r="J37">
+        <v>180</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>0.14586876170049859</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2017,18 +2098,72 @@
       <c r="A43" t="s">
         <v>60</v>
       </c>
-      <c r="L43" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B43">
+        <v>20231126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>132</v>
+      </c>
+      <c r="F43">
+        <v>158</v>
+      </c>
+      <c r="G43">
+        <v>135</v>
+      </c>
+      <c r="H43">
+        <v>124</v>
+      </c>
+      <c r="I43">
+        <v>141</v>
+      </c>
+      <c r="J43">
+        <v>134</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>8.3869672539665027E-2</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
-      <c r="L44" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B44">
+        <v>20231126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>259</v>
+      </c>
+      <c r="F44">
+        <v>251</v>
+      </c>
+      <c r="G44">
+        <v>282</v>
+      </c>
+      <c r="H44">
+        <v>258</v>
+      </c>
+      <c r="I44">
+        <v>238</v>
+      </c>
+      <c r="J44">
+        <v>230</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>7.2019237779796838E-2</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2251,9 +2386,36 @@
       <c r="A51" t="s">
         <v>67</v>
       </c>
-      <c r="L51" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B51">
+        <v>20231126</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>179</v>
+      </c>
+      <c r="F51">
+        <v>169</v>
+      </c>
+      <c r="G51">
+        <v>192</v>
+      </c>
+      <c r="H51">
+        <v>178</v>
+      </c>
+      <c r="I51">
+        <v>213</v>
+      </c>
+      <c r="J51">
+        <v>191</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>8.2359885810389111E-2</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -2677,9 +2839,36 @@
       <c r="A65" t="s">
         <v>80</v>
       </c>
-      <c r="L65" t="e">
+      <c r="B65">
+        <v>20231126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>134</v>
+      </c>
+      <c r="F65">
+        <v>128</v>
+      </c>
+      <c r="G65">
+        <v>128</v>
+      </c>
+      <c r="H65">
+        <v>126</v>
+      </c>
+      <c r="I65">
+        <v>106</v>
+      </c>
+      <c r="J65">
+        <v>124</v>
+      </c>
+      <c r="L65">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>7.708882074563278E-2</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -3199,9 +3388,36 @@
       <c r="A84" t="s">
         <v>97</v>
       </c>
-      <c r="L84" t="e">
+      <c r="B84">
+        <v>20231126</v>
+      </c>
+      <c r="C84" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84">
+        <v>184</v>
+      </c>
+      <c r="F84">
+        <v>177</v>
+      </c>
+      <c r="G84">
+        <v>223</v>
+      </c>
+      <c r="H84">
+        <v>220</v>
+      </c>
+      <c r="I84">
+        <v>222</v>
+      </c>
+      <c r="J84">
+        <v>201</v>
+      </c>
+      <c r="L84">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>9.9676367289190757E-2</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated cell density data
</commit_message>
<xml_diff>
--- a/data/physiology/cell_density/cells.xlsx
+++ b/data/physiology/cell_density/cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/physiology/cell_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC869CC-576C-5547-8A6B-A04A1AD34CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C89E7-C338-FD4A-BC81-EE65D9F28DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="760" windowWidth="18400" windowHeight="17580" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
+    <workbookView xWindow="700" yWindow="760" windowWidth="17320" windowHeight="17620" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
   <si>
     <t>Notes</t>
   </si>
@@ -705,8 +705,8 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,9 +1054,36 @@
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="L11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B11">
+        <v>20231203</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>567</v>
+      </c>
+      <c r="F11">
+        <v>560</v>
+      </c>
+      <c r="G11">
+        <v>565</v>
+      </c>
+      <c r="H11">
+        <v>612</v>
+      </c>
+      <c r="I11">
+        <v>567</v>
+      </c>
+      <c r="J11">
+        <v>620</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>4.5904769150004056E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2713,9 +2740,36 @@
       <c r="A60" t="s">
         <v>76</v>
       </c>
-      <c r="L60" t="e">
+      <c r="B60">
+        <v>20231203</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>111</v>
+      </c>
+      <c r="F60">
+        <v>94</v>
+      </c>
+      <c r="G60">
+        <v>101</v>
+      </c>
+      <c r="H60">
+        <v>97</v>
+      </c>
+      <c r="I60">
+        <v>85</v>
+      </c>
+      <c r="J60">
+        <v>81</v>
+      </c>
+      <c r="L60">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.11482072617995367</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2875,27 +2929,108 @@
       <c r="A66" t="s">
         <v>81</v>
       </c>
-      <c r="L66" t="e">
+      <c r="B66">
+        <v>20231203</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>211</v>
+      </c>
+      <c r="F66">
+        <v>201</v>
+      </c>
+      <c r="G66">
+        <v>235</v>
+      </c>
+      <c r="H66">
+        <v>239</v>
+      </c>
+      <c r="I66">
+        <v>247</v>
+      </c>
+      <c r="J66">
+        <v>289</v>
+      </c>
+      <c r="L66">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.13051554382569588</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>82</v>
       </c>
-      <c r="L67" t="e">
+      <c r="B67">
+        <v>20231203</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>152</v>
+      </c>
+      <c r="F67">
+        <v>150</v>
+      </c>
+      <c r="G67">
+        <v>141</v>
+      </c>
+      <c r="H67">
+        <v>121</v>
+      </c>
+      <c r="I67">
+        <v>150</v>
+      </c>
+      <c r="J67">
+        <v>185</v>
+      </c>
+      <c r="L67">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.13842353495559515</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>83</v>
       </c>
-      <c r="L68" t="e">
+      <c r="B68">
+        <v>20231203</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>187</v>
+      </c>
+      <c r="F68">
+        <v>178</v>
+      </c>
+      <c r="G68">
+        <v>183</v>
+      </c>
+      <c r="H68">
+        <v>206</v>
+      </c>
+      <c r="I68">
+        <v>178</v>
+      </c>
+      <c r="J68">
+        <v>180</v>
+      </c>
+      <c r="L68">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>5.7677475369970629E-2</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -3146,7 +3281,7 @@
         <v>137</v>
       </c>
       <c r="L75">
-        <f t="shared" si="4"/>
+        <f>STDEV(E75:J75)/AVERAGE(E75:J75)</f>
         <v>0.16184485082698888</v>
       </c>
     </row>
@@ -3154,9 +3289,36 @@
       <c r="A76" t="s">
         <v>90</v>
       </c>
-      <c r="L76" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="B76">
+        <v>20231203</v>
+      </c>
+      <c r="C76" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>278</v>
+      </c>
+      <c r="F76">
+        <v>235</v>
+      </c>
+      <c r="G76">
+        <v>240</v>
+      </c>
+      <c r="H76">
+        <v>268</v>
+      </c>
+      <c r="I76">
+        <v>256</v>
+      </c>
+      <c r="J76">
+        <v>262</v>
+      </c>
+      <c r="L76">
+        <f t="shared" ref="L76:L91" si="5">STDEV(E76:J76)/AVERAGE(E76:J76)</f>
+        <v>6.4286122917964872E-2</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
@@ -3191,7 +3353,7 @@
         <v>112</v>
       </c>
       <c r="L77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.10729815265965958</v>
       </c>
     </row>
@@ -3199,9 +3361,36 @@
       <c r="A78" t="s">
         <v>91</v>
       </c>
-      <c r="L78" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="B78">
+        <v>20231203</v>
+      </c>
+      <c r="C78" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>140</v>
+      </c>
+      <c r="F78">
+        <v>168</v>
+      </c>
+      <c r="G78">
+        <v>141</v>
+      </c>
+      <c r="H78">
+        <v>166</v>
+      </c>
+      <c r="I78">
+        <v>163</v>
+      </c>
+      <c r="J78">
+        <v>149</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="5"/>
+        <v>8.2355942290834885E-2</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -3236,7 +3425,7 @@
         <v>141</v>
       </c>
       <c r="L79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.5998331660764032E-2</v>
       </c>
     </row>
@@ -3272,7 +3461,7 @@
         <v>163</v>
       </c>
       <c r="L80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11901536741848444</v>
       </c>
     </row>
@@ -3308,7 +3497,7 @@
         <v>178</v>
       </c>
       <c r="L81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.10534686366530677</v>
       </c>
     </row>
@@ -3344,7 +3533,7 @@
         <v>222</v>
       </c>
       <c r="L82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12101283424380715</v>
       </c>
     </row>
@@ -3380,7 +3569,7 @@
         <v>174</v>
       </c>
       <c r="L83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.15947578484383507</v>
       </c>
     </row>
@@ -3416,7 +3605,7 @@
         <v>201</v>
       </c>
       <c r="L84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.9676367289190757E-2</v>
       </c>
     </row>
@@ -3452,7 +3641,7 @@
         <v>189</v>
       </c>
       <c r="L85">
-        <f t="shared" ref="L85" si="5">STDEV(E85:J85)/AVERAGE(E85:J85)</f>
+        <f t="shared" si="5"/>
         <v>3.5990774094480579E-2</v>
       </c>
     </row>
@@ -3488,7 +3677,7 @@
         <v>176</v>
       </c>
       <c r="L86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.9725341235627082E-2</v>
       </c>
     </row>
@@ -3524,7 +3713,7 @@
         <v>119</v>
       </c>
       <c r="L87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.9641634590415261E-2</v>
       </c>
     </row>
@@ -3560,7 +3749,7 @@
         <v>138</v>
       </c>
       <c r="L88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14788515972771957</v>
       </c>
     </row>
@@ -3569,7 +3758,7 @@
         <v>101</v>
       </c>
       <c r="L89" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3577,9 +3766,36 @@
       <c r="A90" t="s">
         <v>102</v>
       </c>
-      <c r="L90" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+      <c r="B90">
+        <v>20231203</v>
+      </c>
+      <c r="C90" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90">
+        <v>192</v>
+      </c>
+      <c r="F90">
+        <v>189</v>
+      </c>
+      <c r="G90">
+        <v>191</v>
+      </c>
+      <c r="H90">
+        <v>190</v>
+      </c>
+      <c r="I90">
+        <v>189</v>
+      </c>
+      <c r="J90">
+        <v>166</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="5"/>
+        <v>5.3437059088729394E-2</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
@@ -3614,7 +3830,7 @@
         <v>347</v>
       </c>
       <c r="L91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14914954435482167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated analysis with all cell density data recorded
</commit_message>
<xml_diff>
--- a/data/physiology/cell_density/cells.xlsx
+++ b/data/physiology/cell_density/cells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/physiology/cell_density/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C89E7-C338-FD4A-BC81-EE65D9F28DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE584D94-498B-5D44-B314-267E03DADB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="760" windowWidth="17320" windowHeight="17620" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="17320" windowHeight="17620" xr2:uid="{29CB5171-E4B9-8B4B-B84F-0546595A75E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
   <si>
     <t>Notes</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>counted all symbionts</t>
+  </si>
+  <si>
+    <t>Accidentally recorded as POC-R22; actually ACR-R22</t>
   </si>
 </sst>
 </file>
@@ -386,8 +389,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,8 +709,8 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,9 +761,36 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="e">
+      <c r="B2">
+        <v>20231204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>261</v>
+      </c>
+      <c r="F2">
+        <v>256</v>
+      </c>
+      <c r="G2">
+        <v>220</v>
+      </c>
+      <c r="H2">
+        <v>234</v>
+      </c>
+      <c r="I2">
+        <v>240</v>
+      </c>
+      <c r="J2">
+        <v>221</v>
+      </c>
+      <c r="L2">
         <f t="shared" ref="L2:L57" si="0">STDEV(E2:J2)/AVERAGE(E2:J2)</f>
-        <v>#DIV/0!</v>
+        <v>7.2167657445607894E-2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1090,9 +1121,36 @@
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="L12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B12">
+        <v>20231204</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>125</v>
+      </c>
+      <c r="F12">
+        <v>107</v>
+      </c>
+      <c r="G12">
+        <v>103</v>
+      </c>
+      <c r="H12">
+        <v>123</v>
+      </c>
+      <c r="I12">
+        <v>130</v>
+      </c>
+      <c r="J12">
+        <v>121</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>9.0580383257819475E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1171,9 +1229,36 @@
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="L15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B15">
+        <v>20231204</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>294</v>
+      </c>
+      <c r="F15">
+        <v>250</v>
+      </c>
+      <c r="G15">
+        <v>252</v>
+      </c>
+      <c r="H15">
+        <v>315</v>
+      </c>
+      <c r="I15">
+        <v>320</v>
+      </c>
+      <c r="J15">
+        <v>258</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.11429119012942303</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1428,13 +1513,43 @@
         <v>0.23827249330995171</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L23" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B23" s="1">
+        <v>20231119</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>280</v>
+      </c>
+      <c r="F23" s="1">
+        <v>325</v>
+      </c>
+      <c r="G23" s="1">
+        <v>260</v>
+      </c>
+      <c r="H23" s="1">
+        <v>269</v>
+      </c>
+      <c r="I23" s="1">
+        <v>311</v>
+      </c>
+      <c r="J23" s="1">
+        <v>301</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L23" s="1">
+        <f>STDEV(E23:J23)/AVERAGE(E23:J23)</f>
+        <v>8.723379711878837E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2517,40 +2632,40 @@
         <v>0.11284382043625998</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B54">
-        <v>20231119</v>
-      </c>
-      <c r="C54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-      <c r="E54">
-        <v>280</v>
-      </c>
-      <c r="F54">
-        <v>325</v>
-      </c>
-      <c r="G54">
-        <v>260</v>
-      </c>
-      <c r="H54">
-        <v>269</v>
-      </c>
-      <c r="I54">
-        <v>311</v>
-      </c>
-      <c r="J54">
-        <v>301</v>
-      </c>
-      <c r="L54">
+      <c r="B54" s="1">
+        <v>20231204</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>206</v>
+      </c>
+      <c r="F54" s="1">
+        <v>199</v>
+      </c>
+      <c r="G54" s="1">
+        <v>217</v>
+      </c>
+      <c r="H54" s="1">
+        <v>209</v>
+      </c>
+      <c r="I54" s="1">
+        <v>229</v>
+      </c>
+      <c r="J54" s="1">
+        <v>243</v>
+      </c>
+      <c r="L54" s="1">
         <f t="shared" ref="L54" si="3">STDEV(E54:J54)/AVERAGE(E54:J54)</f>
-        <v>8.723379711878837E-2</v>
+        <v>7.5068387883100121E-2</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -2696,7 +2811,7 @@
         <v>152</v>
       </c>
       <c r="L58">
-        <f t="shared" ref="L58:L91" si="4">STDEV(E58:J58)/AVERAGE(E58:J58)</f>
+        <f t="shared" ref="L58:L74" si="4">STDEV(E58:J58)/AVERAGE(E58:J58)</f>
         <v>0.10576651333842681</v>
       </c>
     </row>
@@ -2776,9 +2891,36 @@
       <c r="A61" t="s">
         <v>77</v>
       </c>
-      <c r="L61" t="e">
+      <c r="B61">
+        <v>20231204</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>115</v>
+      </c>
+      <c r="F61">
+        <v>137</v>
+      </c>
+      <c r="G61">
+        <v>111</v>
+      </c>
+      <c r="H61">
+        <v>130</v>
+      </c>
+      <c r="I61">
+        <v>108</v>
+      </c>
+      <c r="J61">
+        <v>123</v>
+      </c>
+      <c r="L61">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>9.4149871399517304E-2</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3757,9 +3899,36 @@
       <c r="A89" t="s">
         <v>101</v>
       </c>
-      <c r="L89" t="e">
+      <c r="B89">
+        <v>20231204</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>149</v>
+      </c>
+      <c r="F89">
+        <v>144</v>
+      </c>
+      <c r="G89">
+        <v>151</v>
+      </c>
+      <c r="H89">
+        <v>158</v>
+      </c>
+      <c r="I89">
+        <v>129</v>
+      </c>
+      <c r="J89">
+        <v>137</v>
+      </c>
+      <c r="L89">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>7.192484060876192E-2</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>